<commit_message>
Almost final version of Presentation: \n Todo: Make Gant-Diagramm #26
</commit_message>
<xml_diff>
--- a/Diplomarbeit/doc/Kampl/Hardware.xlsx
+++ b/Diplomarbeit/doc/Kampl/Hardware.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\Contrude\Diplomarbeit\doc\Kampl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51144A87-F21B-4B0C-9FE8-8F00F3227FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F108E6-2AA2-43D2-82A9-E253A2BF2201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{F8F58720-A04D-47BF-B44C-22AB8B67CE72}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{F8F58720-A04D-47BF-B44C-22AB8B67CE72}"/>
   </bookViews>
   <sheets>
     <sheet name="Anforderungen" sheetId="1" r:id="rId1"/>
@@ -523,6 +523,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -532,11 +537,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Link" xfId="2" builtinId="8"/>
@@ -1832,7 +1832,7 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="B2:K20"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" zoomScale="131" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="95" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1852,18 +1852,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="31.8" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="32"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="37"/>
     </row>
     <row r="3" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B3" s="3" t="s">
@@ -2200,8 +2200,8 @@
   <sheetPr codeName="Tabelle4"/>
   <dimension ref="B1:XFD43"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="117" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -2253,7 +2253,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:5 16384:16384" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5 16384:16384" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="D3" s="23" t="s">
         <v>13</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>13.89</v>
       </c>
     </row>
-    <row r="4" spans="2:5 16384:16384" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5 16384:16384" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="D4" s="23" t="s">
         <v>16</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="5" spans="2:5 16384:16384" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5 16384:16384" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="D5" s="23" t="s">
         <v>31</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>2.72</v>
       </c>
     </row>
-    <row r="6" spans="2:5 16384:16384" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5 16384:16384" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="D6" s="23" t="s">
         <v>22</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="7" spans="2:5 16384:16384" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
       <c r="D7" s="22" t="s">
         <v>41</v>
       </c>
@@ -2686,7 +2686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B17159C8-8BAF-4669-BFDA-DD3C1645E6A5}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
+    <sheetView zoomScale="70" workbookViewId="0">
       <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
@@ -2696,37 +2696,37 @@
     <col min="2" max="2" width="22.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:6" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-    </row>
-    <row r="2" spans="1:6" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="36" t="s">
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+    </row>
+    <row r="2" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="33" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2791,10 +2791,10 @@
       <c r="F7" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="37"/>
+      <c r="B9" s="34"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">

</xml_diff>

<commit_message>
Second Thesis Presentation #51
</commit_message>
<xml_diff>
--- a/Diplomarbeit/doc/Kampl/Hardware.xlsx
+++ b/Diplomarbeit/doc/Kampl/Hardware.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\Contrude\Diplomarbeit\doc\Kampl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maximilian\Desktop\Contrude\Diplomarbeit\doc\Kampl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F67402-03B5-43BD-A771-400E2FABBDC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB1D8EB-EBA4-46DA-B16F-77E728300EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{F8F58720-A04D-47BF-B44C-22AB8B67CE72}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{F8F58720-A04D-47BF-B44C-22AB8B67CE72}"/>
   </bookViews>
   <sheets>
     <sheet name="Anforderungen" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Stromverbrauch" sheetId="6" r:id="rId3"/>
     <sheet name="Hülle" sheetId="5" r:id="rId4"/>
     <sheet name="Links" sheetId="7" r:id="rId5"/>
+    <sheet name="Tatsächliche Kosten" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="99">
   <si>
     <t>Auflagen</t>
   </si>
@@ -325,6 +326,18 @@
   </si>
   <si>
     <t>Tage</t>
+  </si>
+  <si>
+    <t>GY-521</t>
+  </si>
+  <si>
+    <t>F2F Kabel</t>
+  </si>
+  <si>
+    <t>Esp32</t>
+  </si>
+  <si>
+    <t>Summe</t>
   </si>
 </sst>
 </file>
@@ -332,10 +345,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -375,6 +388,28 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -568,32 +603,32 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -607,6 +642,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -616,9 +657,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Link" xfId="2" builtinId="8"/>
@@ -1915,39 +1953,39 @@
   <dimension ref="B2:K20"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="95" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" customWidth="1"/>
-    <col min="2" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.88671875" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="31.8" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B2" s="35" t="s">
+    <row r="2" spans="2:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="37"/>
-    </row>
-    <row r="3" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="43"/>
+    </row>
+    <row r="3" spans="2:11" ht="24" x14ac:dyDescent="0.4">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1979,7 +2017,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
@@ -2012,7 +2050,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
@@ -2044,7 +2082,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
@@ -2076,7 +2114,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
@@ -2108,7 +2146,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
@@ -2140,7 +2178,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
@@ -2172,14 +2210,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G10" s="7"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D12" s="11"/>
     </row>
-    <row r="13" spans="2:11" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="13" spans="2:11" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
@@ -2191,7 +2229,7 @@
       <c r="J13" s="18"/>
       <c r="K13" s="18"/>
     </row>
-    <row r="14" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:11" ht="24" x14ac:dyDescent="0.4">
       <c r="B14" s="12"/>
       <c r="C14" t="s">
         <v>73</v>
@@ -2205,21 +2243,21 @@
       <c r="J14" s="14"/>
       <c r="K14" s="12"/>
     </row>
-    <row r="15" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B15" s="15"/>
       <c r="C15" s="16"/>
       <c r="D15" s="17"/>
       <c r="F15" s="16"/>
       <c r="I15" s="16"/>
     </row>
-    <row r="16" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B16" s="15"/>
       <c r="C16" s="16"/>
       <c r="D16" s="17"/>
       <c r="F16" s="16"/>
       <c r="I16" s="16"/>
     </row>
-    <row r="17" spans="2:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B17" s="15"/>
       <c r="C17" s="16"/>
       <c r="D17" s="17"/>
@@ -2227,7 +2265,7 @@
       <c r="I17" s="16"/>
       <c r="J17" s="17"/>
     </row>
-    <row r="18" spans="2:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B18" s="15"/>
       <c r="C18" s="16"/>
       <c r="D18" s="17"/>
@@ -2235,7 +2273,7 @@
       <c r="I18" s="16"/>
       <c r="J18" s="17"/>
     </row>
-    <row r="19" spans="2:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B19" s="15"/>
       <c r="C19" s="16"/>
       <c r="D19" s="17"/>
@@ -2243,7 +2281,7 @@
       <c r="I19" s="16"/>
       <c r="J19" s="17"/>
     </row>
-    <row r="20" spans="2:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B20" s="15"/>
       <c r="C20" s="16"/>
       <c r="D20" s="17"/>
@@ -2288,30 +2326,30 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.44140625" style="22" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" style="22" customWidth="1"/>
     <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:6 16384:16384" x14ac:dyDescent="0.25">
       <c r="B1" s="24" t="s">
         <v>43</v>
       </c>
@@ -2323,7 +2361,7 @@
       </c>
       <c r="E1" s="19"/>
     </row>
-    <row r="2" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6 16384:16384" x14ac:dyDescent="0.25">
       <c r="B2" s="1">
         <v>1</v>
       </c>
@@ -2337,7 +2375,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:5 16384:16384" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D3" s="23" t="s">
         <v>13</v>
       </c>
@@ -2345,48 +2383,60 @@
         <f xml:space="preserve"> 9.9+3.99</f>
         <v>13.89</v>
       </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
       <c r="XFD3" s="10">
         <f t="shared" ref="XFD3:XFD8" si="0">SUM(E3:XFC3)</f>
-        <v>13.89</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5 16384:16384" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>14.89</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D4" s="23" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="8">
         <v>1.1100000000000001</v>
       </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
       <c r="XFD4" s="10">
         <f t="shared" si="0"/>
-        <v>1.1100000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5 16384:16384" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>4.1100000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D5" s="23" t="s">
         <v>31</v>
       </c>
       <c r="E5" s="8">
         <v>2.72</v>
       </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
       <c r="XFD5" s="10">
         <f t="shared" si="0"/>
-        <v>2.72</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5 16384:16384" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>3.72</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D6" s="23" t="s">
         <v>22</v>
       </c>
       <c r="E6" s="6">
         <v>5.9</v>
       </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
       <c r="XFD6" s="10">
         <f t="shared" si="0"/>
-        <v>5.9</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6 16384:16384" x14ac:dyDescent="0.25">
       <c r="D7" s="22" t="s">
         <v>41</v>
       </c>
@@ -2399,7 +2449,7 @@
         <v>23.619999999999997</v>
       </c>
     </row>
-    <row r="8" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6 16384:16384" x14ac:dyDescent="0.25">
       <c r="D8" s="22" t="s">
         <v>40</v>
       </c>
@@ -2412,7 +2462,7 @@
         <v>70.859999999999985</v>
       </c>
     </row>
-    <row r="9" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6 16384:16384" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>2</v>
       </c>
@@ -2426,7 +2476,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:5 16384:16384" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C10" s="21"/>
       <c r="D10" s="23" t="s">
         <v>13</v>
@@ -2436,7 +2486,7 @@
         <v>13.89</v>
       </c>
     </row>
-    <row r="11" spans="2:5 16384:16384" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D11" s="4" t="s">
         <v>51</v>
       </c>
@@ -2444,7 +2494,7 @@
         <v>9.06</v>
       </c>
     </row>
-    <row r="12" spans="2:5 16384:16384" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D12" s="23" t="s">
         <v>31</v>
       </c>
@@ -2452,7 +2502,7 @@
         <v>2.72</v>
       </c>
     </row>
-    <row r="13" spans="2:5 16384:16384" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D13" s="23" t="s">
         <v>22</v>
       </c>
@@ -2460,7 +2510,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="14" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6 16384:16384" x14ac:dyDescent="0.25">
       <c r="D14" s="22" t="s">
         <v>41</v>
       </c>
@@ -2469,7 +2519,7 @@
         <v>31.57</v>
       </c>
     </row>
-    <row r="15" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6 16384:16384" x14ac:dyDescent="0.25">
       <c r="D15" s="22" t="s">
         <v>40</v>
       </c>
@@ -2478,7 +2528,7 @@
         <v>94.710000000000008</v>
       </c>
     </row>
-    <row r="16" spans="2:5 16384:16384" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6 16384:16384" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>3</v>
       </c>
@@ -2492,7 +2542,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D17" s="4" t="s">
         <v>18</v>
       </c>
@@ -2500,7 +2550,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="18" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D18" s="23" t="s">
         <v>16</v>
       </c>
@@ -2508,7 +2558,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="19" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D19" s="23" t="s">
         <v>31</v>
       </c>
@@ -2516,7 +2566,7 @@
         <v>2.72</v>
       </c>
     </row>
-    <row r="20" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D20" s="23" t="s">
         <v>22</v>
       </c>
@@ -2524,7 +2574,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D21" s="22" t="s">
         <v>41</v>
       </c>
@@ -2533,7 +2583,7 @@
         <v>26.229999999999997</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D22" s="22" t="s">
         <v>40</v>
       </c>
@@ -2542,7 +2592,7 @@
         <v>78.69</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>4</v>
       </c>
@@ -2556,7 +2606,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D24" s="4" t="s">
         <v>18</v>
       </c>
@@ -2564,7 +2614,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="25" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D25" s="4" t="s">
         <v>51</v>
       </c>
@@ -2572,7 +2622,7 @@
         <v>9.06</v>
       </c>
     </row>
-    <row r="26" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D26" s="23" t="s">
         <v>31</v>
       </c>
@@ -2580,7 +2630,7 @@
         <v>2.72</v>
       </c>
     </row>
-    <row r="27" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D27" s="23" t="s">
         <v>22</v>
       </c>
@@ -2588,7 +2638,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D28" s="22" t="s">
         <v>41</v>
       </c>
@@ -2597,7 +2647,7 @@
         <v>34.18</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D29" s="22" t="s">
         <v>40</v>
       </c>
@@ -2606,7 +2656,7 @@
         <v>102.53999999999999</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>5</v>
       </c>
@@ -2620,7 +2670,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D31" s="4" t="s">
         <v>36</v>
       </c>
@@ -2628,7 +2678,7 @@
         <v>29.75</v>
       </c>
     </row>
-    <row r="32" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D32" s="4" t="s">
         <v>16</v>
       </c>
@@ -2636,7 +2686,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="33" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D33" s="23" t="s">
         <v>31</v>
       </c>
@@ -2644,7 +2694,7 @@
         <v>2.72</v>
       </c>
     </row>
-    <row r="34" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D34" s="23" t="s">
         <v>22</v>
       </c>
@@ -2652,7 +2702,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D35" s="22" t="s">
         <v>41</v>
       </c>
@@ -2661,7 +2711,7 @@
         <v>39.479999999999997</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D36" s="22" t="s">
         <v>40</v>
       </c>
@@ -2670,7 +2720,7 @@
         <v>118.44</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="1">
         <v>6</v>
       </c>
@@ -2684,7 +2734,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D38" s="4" t="s">
         <v>36</v>
       </c>
@@ -2692,7 +2742,7 @@
         <v>29.75</v>
       </c>
     </row>
-    <row r="39" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D39" s="4" t="s">
         <v>51</v>
       </c>
@@ -2700,7 +2750,7 @@
         <v>9.06</v>
       </c>
     </row>
-    <row r="40" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D40" s="23" t="s">
         <v>31</v>
       </c>
@@ -2708,7 +2758,7 @@
         <v>2.72</v>
       </c>
     </row>
-    <row r="41" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D41" s="23" t="s">
         <v>22</v>
       </c>
@@ -2716,7 +2766,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D42" s="22" t="s">
         <v>41</v>
       </c>
@@ -2725,7 +2775,7 @@
         <v>47.43</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D43" s="22" t="s">
         <v>40</v>
       </c>
@@ -2774,17 +2824,17 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="19.44140625" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>74</v>
       </c>
@@ -2794,12 +2844,8 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>75</v>
@@ -2813,12 +2859,8 @@
       <c r="E3" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>13</v>
@@ -2833,12 +2875,8 @@
         <f>C4*D4</f>
         <v>0.65</v>
       </c>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-    </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
@@ -2852,13 +2890,13 @@
         <f>C5*D5</f>
         <v>0.33500000000000002</v>
       </c>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="39"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5" s="36"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>77</v>
@@ -2873,12 +2911,8 @@
         <f>C6*D6</f>
         <v>2.5999999999999998E-4</v>
       </c>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>78</v>
@@ -2890,15 +2924,11 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" ref="E6:E7" si="0">C7*D7</f>
+        <f t="shared" ref="E7" si="0">C7*D7</f>
         <v>1.384E-2</v>
       </c>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>85</v>
       </c>
@@ -2906,12 +2936,8 @@
         <f>SUM(E4:E7)</f>
         <v>0.9991000000000001</v>
       </c>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E9">
         <v>0.2</v>
       </c>
@@ -2919,7 +2945,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>86</v>
       </c>
@@ -2928,7 +2954,7 @@
         <v>9.9910000000000016E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>87</v>
       </c>
@@ -2937,7 +2963,7 @@
         <v>2.39784E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>88</v>
       </c>
@@ -2946,7 +2972,7 @@
         <v>0.16784880000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>89</v>
       </c>
@@ -2955,7 +2981,7 @@
         <v>0.71935199999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>90</v>
       </c>
@@ -2966,7 +2992,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>91</v>
       </c>
@@ -2978,7 +3004,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18">
         <f>B17/24</f>
         <v>35.416666666666664</v>
@@ -3000,13 +3026,13 @@
       <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="30" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
         <v>53</v>
       </c>
@@ -3020,7 +3046,7 @@
       <c r="E1" s="32"/>
       <c r="F1" s="32"/>
     </row>
-    <row r="2" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>52</v>
       </c>
@@ -3040,7 +3066,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>54</v>
       </c>
@@ -3052,7 +3078,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>56</v>
       </c>
@@ -3064,7 +3090,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>57</v>
       </c>
@@ -3076,7 +3102,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>58</v>
       </c>
@@ -3088,7 +3114,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>61</v>
       </c>
@@ -3100,13 +3126,13 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
         <v>62</v>
       </c>
       <c r="B9" s="34"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -3114,7 +3140,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -3122,7 +3148,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>3</v>
       </c>
@@ -3130,7 +3156,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>4</v>
       </c>
@@ -3138,7 +3164,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>5</v>
       </c>
@@ -3146,7 +3172,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>6</v>
       </c>
@@ -3154,7 +3180,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>7</v>
       </c>
@@ -3162,7 +3188,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>8</v>
       </c>
@@ -3170,7 +3196,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>9</v>
       </c>
@@ -3178,7 +3204,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>10</v>
       </c>
@@ -3200,19 +3226,19 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="38" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="35" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="38" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>84</v>
       </c>
@@ -3224,4 +3250,71 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493E053C-96E9-4B54-B663-4984A59DE940}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" style="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="39" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.42578125" style="37"/>
+    <col min="5" max="5" width="12.140625" style="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="37"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="39">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="39">
+        <v>12.03</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="39">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="39">
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D9" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="E9" s="39">
+        <f>SUM(B:B)</f>
+        <v>35.28</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{D451895C-5A8E-4860-AA30-36B04BA01438}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{718F6AB7-D945-427E-85D0-B6D3520F9D42}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Temporary Final Version #51
</commit_message>
<xml_diff>
--- a/Diplomarbeit/doc/Kampl/Hardware.xlsx
+++ b/Diplomarbeit/doc/Kampl/Hardware.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maximilian\Desktop\Contrude\Diplomarbeit\doc\Kampl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB1D8EB-EBA4-46DA-B16F-77E728300EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA4278C-A88B-42F1-9CBF-F4F21C6C7588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{F8F58720-A04D-47BF-B44C-22AB8B67CE72}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="16200" activeTab="5" xr2:uid="{F8F58720-A04D-47BF-B44C-22AB8B67CE72}"/>
   </bookViews>
   <sheets>
     <sheet name="Anforderungen" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="109">
   <si>
     <t>Auflagen</t>
   </si>
@@ -331,13 +331,43 @@
     <t>GY-521</t>
   </si>
   <si>
-    <t>F2F Kabel</t>
-  </si>
-  <si>
-    <t>Esp32</t>
-  </si>
-  <si>
-    <t>Summe</t>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>Anzahl</t>
+  </si>
+  <si>
+    <t>Ort</t>
+  </si>
+  <si>
+    <t>Produkt</t>
+  </si>
+  <si>
+    <t>Ali-Express</t>
+  </si>
+  <si>
+    <t>Einzelpreis</t>
+  </si>
+  <si>
+    <t>Lieferkosten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preis gesamt </t>
+  </si>
+  <si>
+    <t>ET-Starterkit</t>
+  </si>
+  <si>
+    <t>Preis insgesamt</t>
+  </si>
+  <si>
+    <t>Preis/Person</t>
+  </si>
+  <si>
+    <t>Preis/Person (-ET_Starterkit)</t>
+  </si>
+  <si>
+    <t>Preis (-ET_Starterkit)</t>
   </si>
 </sst>
 </file>
@@ -348,7 +378,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -394,29 +424,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="16"/>
-      <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="16"/>
-      <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -459,8 +474,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -600,13 +627,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -644,10 +693,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -657,6 +703,26 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Link" xfId="2" builtinId="8"/>
@@ -1972,18 +2038,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="43"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="40"/>
     </row>
     <row r="3" spans="2:11" ht="24" x14ac:dyDescent="0.4">
       <c r="B3" s="3" t="s">
@@ -2820,7 +2886,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56374579-2866-471D-B3A1-5191C1903E48}">
   <dimension ref="A2:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="183" zoomScaleNormal="177" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="183" zoomScaleNormal="177" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -3254,67 +3320,200 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493E053C-96E9-4B54-B663-4984A59DE940}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.140625" style="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="39" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.42578125" style="37"/>
-    <col min="5" max="5" width="12.140625" style="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="37"/>
+    <col min="1" max="1" width="9.28515625" style="41" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" style="41" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" style="42" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="44" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="44" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.7109375" style="44" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="37"/>
+    <col min="8" max="8" width="9.140625" style="37" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" style="37" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F1" s="43"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="59" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="60" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="60" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="60" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="45">
+        <v>3</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="47">
+        <v>3.19</v>
+      </c>
+      <c r="E3" s="47">
+        <f>12.03-9.57</f>
+        <v>2.4599999999999991</v>
+      </c>
+      <c r="F3" s="47">
+        <f>(D3*A3)+E3</f>
+        <v>12.03</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="45">
+        <v>3</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="47">
+        <f>10.40833/A4</f>
+        <v>3.469443333333333</v>
+      </c>
+      <c r="E4" s="47">
+        <f>3.25+2.73</f>
+        <v>5.98</v>
+      </c>
+      <c r="F4" s="47">
+        <f t="shared" ref="F4:F5" si="0">(D4*A4)+E4</f>
+        <v>16.38833</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="45">
+        <v>3</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="39">
-        <v>6.7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="39">
-        <v>12.03</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="B3" s="39">
-        <v>2.95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="38" t="s">
-        <v>97</v>
-      </c>
-      <c r="B4" s="39">
-        <v>13.6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D9" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="E9" s="39">
-        <f>SUM(B:B)</f>
-        <v>35.28</v>
+      <c r="D5" s="47">
+        <f>7.49/A5</f>
+        <v>2.4966666666666666</v>
+      </c>
+      <c r="E5" s="47">
+        <f>3.15+2.15</f>
+        <v>5.3</v>
+      </c>
+      <c r="F5" s="47">
+        <f>(D5*A5)+E5</f>
+        <v>12.79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="49">
+        <v>1</v>
+      </c>
+      <c r="B6" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="51">
+        <v>16.13</v>
+      </c>
+      <c r="E6" s="51">
+        <f>F6-D6</f>
+        <v>3.990000000000002</v>
+      </c>
+      <c r="F6" s="51">
+        <v>20.12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="54"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C8" s="52"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+    </row>
+    <row r="9" spans="1:6" s="41" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="57" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="57" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B10" s="48">
+        <f>SUM(F3:F6)</f>
+        <v>61.328329999999994</v>
+      </c>
+      <c r="C10" s="52"/>
+      <c r="D10" s="47">
+        <f>B10/3</f>
+        <v>20.442776666666663</v>
+      </c>
+      <c r="E10" s="53"/>
+      <c r="F10" s="47">
+        <f>SUM(F3:F5)/3</f>
+        <v>13.736109999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C11" s="52"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C12" s="52"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="57" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F13" s="47">
+        <f>SUM(F3:F5)</f>
+        <v>41.208329999999997</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{D451895C-5A8E-4860-AA30-36B04BA01438}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{718F6AB7-D945-427E-85D0-B6D3520F9D42}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated DA-Presentation & Changed pricing
</commit_message>
<xml_diff>
--- a/Diplomarbeit/doc/Kampl/Hardware.xlsx
+++ b/Diplomarbeit/doc/Kampl/Hardware.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maximilian\Desktop\Contrude\Diplomarbeit\doc\Kampl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\Contrude\Diplomarbeit\doc\Kampl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA4278C-A88B-42F1-9CBF-F4F21C6C7588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92FAE9EE-698C-42CB-98AF-9DC302855487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="16200" activeTab="5" xr2:uid="{F8F58720-A04D-47BF-B44C-22AB8B67CE72}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="5" xr2:uid="{F8F58720-A04D-47BF-B44C-22AB8B67CE72}"/>
   </bookViews>
   <sheets>
     <sheet name="Anforderungen" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="114">
   <si>
     <t>Auflagen</t>
   </si>
@@ -358,9 +358,6 @@
     <t>ET-Starterkit</t>
   </si>
   <si>
-    <t>Preis insgesamt</t>
-  </si>
-  <si>
     <t>Preis/Person</t>
   </si>
   <si>
@@ -368,6 +365,24 @@
   </si>
   <si>
     <t>Preis (-ET_Starterkit)</t>
+  </si>
+  <si>
+    <t>Domainkosten</t>
+  </si>
+  <si>
+    <t>Buchdruckkosten</t>
+  </si>
+  <si>
+    <t>Preis Hardware insgesamt</t>
+  </si>
+  <si>
+    <t>Preis ins. (-ET)</t>
+  </si>
+  <si>
+    <t>Preis/Person (-ET)</t>
+  </si>
+  <si>
+    <t>Preis ins.</t>
   </si>
 </sst>
 </file>
@@ -375,8 +390,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -431,7 +446,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -483,6 +498,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.749992370372631"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -652,32 +673,32 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -694,6 +715,23 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -703,26 +741,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Link" xfId="2" builtinId="8"/>
@@ -2022,36 +2042,36 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="38" t="s">
+    <row r="2" spans="2:11" ht="31.8" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B2" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="40"/>
-    </row>
-    <row r="3" spans="2:11" ht="24" x14ac:dyDescent="0.4">
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="57"/>
+    </row>
+    <row r="3" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -2083,7 +2103,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
@@ -2116,7 +2136,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
@@ -2148,7 +2168,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
@@ -2180,7 +2200,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
@@ -2212,7 +2232,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
@@ -2244,7 +2264,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
@@ -2276,14 +2296,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="G10" s="7"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="D12" s="11"/>
     </row>
-    <row r="13" spans="2:11" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="13" spans="2:11" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
@@ -2295,7 +2315,7 @@
       <c r="J13" s="18"/>
       <c r="K13" s="18"/>
     </row>
-    <row r="14" spans="2:11" ht="24" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B14" s="12"/>
       <c r="C14" t="s">
         <v>73</v>
@@ -2309,21 +2329,21 @@
       <c r="J14" s="14"/>
       <c r="K14" s="12"/>
     </row>
-    <row r="15" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B15" s="15"/>
       <c r="C15" s="16"/>
       <c r="D15" s="17"/>
       <c r="F15" s="16"/>
       <c r="I15" s="16"/>
     </row>
-    <row r="16" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B16" s="15"/>
       <c r="C16" s="16"/>
       <c r="D16" s="17"/>
       <c r="F16" s="16"/>
       <c r="I16" s="16"/>
     </row>
-    <row r="17" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B17" s="15"/>
       <c r="C17" s="16"/>
       <c r="D17" s="17"/>
@@ -2331,7 +2351,7 @@
       <c r="I17" s="16"/>
       <c r="J17" s="17"/>
     </row>
-    <row r="18" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B18" s="15"/>
       <c r="C18" s="16"/>
       <c r="D18" s="17"/>
@@ -2339,7 +2359,7 @@
       <c r="I18" s="16"/>
       <c r="J18" s="17"/>
     </row>
-    <row r="19" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="15"/>
       <c r="C19" s="16"/>
       <c r="D19" s="17"/>
@@ -2347,7 +2367,7 @@
       <c r="I19" s="16"/>
       <c r="J19" s="17"/>
     </row>
-    <row r="20" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B20" s="15"/>
       <c r="C20" s="16"/>
       <c r="D20" s="17"/>
@@ -2392,30 +2412,30 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.42578125" style="22" customWidth="1"/>
+    <col min="1" max="1" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.44140625" style="22" customWidth="1"/>
     <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6 16384:16384" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6 16384:16384" x14ac:dyDescent="0.3">
       <c r="B1" s="24" t="s">
         <v>43</v>
       </c>
@@ -2427,7 +2447,7 @@
       </c>
       <c r="E1" s="19"/>
     </row>
-    <row r="2" spans="2:6 16384:16384" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6 16384:16384" x14ac:dyDescent="0.3">
       <c r="B2" s="1">
         <v>1</v>
       </c>
@@ -2441,7 +2461,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="D3" s="23" t="s">
         <v>13</v>
       </c>
@@ -2457,7 +2477,7 @@
         <v>14.89</v>
       </c>
     </row>
-    <row r="4" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="D4" s="23" t="s">
         <v>16</v>
       </c>
@@ -2472,7 +2492,7 @@
         <v>4.1100000000000003</v>
       </c>
     </row>
-    <row r="5" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="D5" s="23" t="s">
         <v>31</v>
       </c>
@@ -2487,7 +2507,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="6" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="D6" s="23" t="s">
         <v>22</v>
       </c>
@@ -2502,7 +2522,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="7" spans="2:6 16384:16384" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6 16384:16384" x14ac:dyDescent="0.3">
       <c r="D7" s="22" t="s">
         <v>41</v>
       </c>
@@ -2515,7 +2535,7 @@
         <v>23.619999999999997</v>
       </c>
     </row>
-    <row r="8" spans="2:6 16384:16384" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6 16384:16384" x14ac:dyDescent="0.3">
       <c r="D8" s="22" t="s">
         <v>40</v>
       </c>
@@ -2528,7 +2548,7 @@
         <v>70.859999999999985</v>
       </c>
     </row>
-    <row r="9" spans="2:6 16384:16384" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6 16384:16384" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>2</v>
       </c>
@@ -2542,7 +2562,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C10" s="21"/>
       <c r="D10" s="23" t="s">
         <v>13</v>
@@ -2552,7 +2572,7 @@
         <v>13.89</v>
       </c>
     </row>
-    <row r="11" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="D11" s="4" t="s">
         <v>51</v>
       </c>
@@ -2560,7 +2580,7 @@
         <v>9.06</v>
       </c>
     </row>
-    <row r="12" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="D12" s="23" t="s">
         <v>31</v>
       </c>
@@ -2568,7 +2588,7 @@
         <v>2.72</v>
       </c>
     </row>
-    <row r="13" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="D13" s="23" t="s">
         <v>22</v>
       </c>
@@ -2576,7 +2596,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="14" spans="2:6 16384:16384" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6 16384:16384" x14ac:dyDescent="0.3">
       <c r="D14" s="22" t="s">
         <v>41</v>
       </c>
@@ -2585,7 +2605,7 @@
         <v>31.57</v>
       </c>
     </row>
-    <row r="15" spans="2:6 16384:16384" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6 16384:16384" x14ac:dyDescent="0.3">
       <c r="D15" s="22" t="s">
         <v>40</v>
       </c>
@@ -2594,7 +2614,7 @@
         <v>94.710000000000008</v>
       </c>
     </row>
-    <row r="16" spans="2:6 16384:16384" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6 16384:16384" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
         <v>3</v>
       </c>
@@ -2608,7 +2628,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="D17" s="4" t="s">
         <v>18</v>
       </c>
@@ -2616,7 +2636,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="18" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="D18" s="23" t="s">
         <v>16</v>
       </c>
@@ -2624,7 +2644,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="19" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="D19" s="23" t="s">
         <v>31</v>
       </c>
@@ -2632,7 +2652,7 @@
         <v>2.72</v>
       </c>
     </row>
-    <row r="20" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="D20" s="23" t="s">
         <v>22</v>
       </c>
@@ -2640,7 +2660,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D21" s="22" t="s">
         <v>41</v>
       </c>
@@ -2649,7 +2669,7 @@
         <v>26.229999999999997</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D22" s="22" t="s">
         <v>40</v>
       </c>
@@ -2658,7 +2678,7 @@
         <v>78.69</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="1">
         <v>4</v>
       </c>
@@ -2672,7 +2692,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="D24" s="4" t="s">
         <v>18</v>
       </c>
@@ -2680,7 +2700,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="25" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="D25" s="4" t="s">
         <v>51</v>
       </c>
@@ -2688,7 +2708,7 @@
         <v>9.06</v>
       </c>
     </row>
-    <row r="26" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="D26" s="23" t="s">
         <v>31</v>
       </c>
@@ -2696,7 +2716,7 @@
         <v>2.72</v>
       </c>
     </row>
-    <row r="27" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="D27" s="23" t="s">
         <v>22</v>
       </c>
@@ -2704,7 +2724,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D28" s="22" t="s">
         <v>41</v>
       </c>
@@ -2713,7 +2733,7 @@
         <v>34.18</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D29" s="22" t="s">
         <v>40</v>
       </c>
@@ -2722,7 +2742,7 @@
         <v>102.53999999999999</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="1">
         <v>5</v>
       </c>
@@ -2736,7 +2756,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="D31" s="4" t="s">
         <v>36</v>
       </c>
@@ -2744,7 +2764,7 @@
         <v>29.75</v>
       </c>
     </row>
-    <row r="32" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="D32" s="4" t="s">
         <v>16</v>
       </c>
@@ -2752,7 +2772,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="33" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="D33" s="23" t="s">
         <v>31</v>
       </c>
@@ -2760,7 +2780,7 @@
         <v>2.72</v>
       </c>
     </row>
-    <row r="34" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="D34" s="23" t="s">
         <v>22</v>
       </c>
@@ -2768,7 +2788,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D35" s="22" t="s">
         <v>41</v>
       </c>
@@ -2777,7 +2797,7 @@
         <v>39.479999999999997</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D36" s="22" t="s">
         <v>40</v>
       </c>
@@ -2786,7 +2806,7 @@
         <v>118.44</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B37" s="1">
         <v>6</v>
       </c>
@@ -2800,7 +2820,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="D38" s="4" t="s">
         <v>36</v>
       </c>
@@ -2808,7 +2828,7 @@
         <v>29.75</v>
       </c>
     </row>
-    <row r="39" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="D39" s="4" t="s">
         <v>51</v>
       </c>
@@ -2816,7 +2836,7 @@
         <v>9.06</v>
       </c>
     </row>
-    <row r="40" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="D40" s="23" t="s">
         <v>31</v>
       </c>
@@ -2824,7 +2844,7 @@
         <v>2.72</v>
       </c>
     </row>
-    <row r="41" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="D41" s="23" t="s">
         <v>22</v>
       </c>
@@ -2832,7 +2852,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D42" s="22" t="s">
         <v>41</v>
       </c>
@@ -2841,7 +2861,7 @@
         <v>47.43</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D43" s="22" t="s">
         <v>40</v>
       </c>
@@ -2890,17 +2910,17 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>74</v>
       </c>
@@ -2911,7 +2931,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>75</v>
@@ -2926,7 +2946,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>13</v>
@@ -2942,7 +2962,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
@@ -2962,7 +2982,7 @@
       <c r="I5"/>
       <c r="J5" s="36"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>77</v>
@@ -2978,7 +2998,7 @@
         <v>2.5999999999999998E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>78</v>
@@ -2994,7 +3014,7 @@
         <v>1.384E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
         <v>85</v>
       </c>
@@ -3003,7 +3023,7 @@
         <v>0.9991000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E9">
         <v>0.2</v>
       </c>
@@ -3011,7 +3031,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>86</v>
       </c>
@@ -3020,7 +3040,7 @@
         <v>9.9910000000000016E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>87</v>
       </c>
@@ -3029,7 +3049,7 @@
         <v>2.39784E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>88</v>
       </c>
@@ -3038,7 +3058,7 @@
         <v>0.16784880000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>89</v>
       </c>
@@ -3047,7 +3067,7 @@
         <v>0.71935199999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>90</v>
       </c>
@@ -3058,7 +3078,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>91</v>
       </c>
@@ -3070,7 +3090,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B18">
         <f>B17/24</f>
         <v>35.416666666666664</v>
@@ -3092,13 +3112,13 @@
       <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="32" t="s">
         <v>53</v>
       </c>
@@ -3112,7 +3132,7 @@
       <c r="E1" s="32"/>
       <c r="F1" s="32"/>
     </row>
-    <row r="2" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
         <v>52</v>
       </c>
@@ -3132,7 +3152,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>54</v>
       </c>
@@ -3144,7 +3164,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>56</v>
       </c>
@@ -3156,7 +3176,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>57</v>
       </c>
@@ -3168,7 +3188,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>58</v>
       </c>
@@ -3180,7 +3200,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>61</v>
       </c>
@@ -3192,13 +3212,13 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="34" t="s">
         <v>62</v>
       </c>
       <c r="B9" s="34"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -3206,7 +3226,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -3214,7 +3234,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>3</v>
       </c>
@@ -3222,7 +3242,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>4</v>
       </c>
@@ -3230,7 +3250,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>5</v>
       </c>
@@ -3238,7 +3258,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>6</v>
       </c>
@@ -3246,7 +3266,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>7</v>
       </c>
@@ -3254,7 +3274,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>8</v>
       </c>
@@ -3262,7 +3282,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>9</v>
       </c>
@@ -3270,7 +3290,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>10</v>
       </c>
@@ -3292,19 +3312,19 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="35" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="35" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>84</v>
       </c>
@@ -3320,197 +3340,231 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493E053C-96E9-4B54-B663-4984A59DE940}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="41" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" style="41" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="42" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" style="44" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="44" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.7109375" style="44" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="37"/>
-    <col min="8" max="8" width="9.140625" style="37" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" style="37" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="37"/>
+    <col min="1" max="1" width="9.33203125" style="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5546875" style="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" style="37" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" style="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" style="40" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35" style="40" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" style="37"/>
+    <col min="8" max="8" width="22.5546875" style="37" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.44140625" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F1" s="43"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="58" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="F1" s="39"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A2" s="52" t="s">
         <v>97</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="D2" s="60" t="s">
+      <c r="D2" s="54" t="s">
         <v>101</v>
       </c>
-      <c r="E2" s="60" t="s">
+      <c r="E2" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="F2" s="60" t="s">
+      <c r="F2" s="54" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="45">
+      <c r="H2" s="58" t="s">
+        <v>108</v>
+      </c>
+      <c r="I2" s="43">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A3" s="41">
         <v>3</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="42" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="47">
+      <c r="D3" s="43">
         <v>3.19</v>
       </c>
-      <c r="E3" s="47">
+      <c r="E3" s="43">
         <f>12.03-9.57</f>
         <v>2.4599999999999991</v>
       </c>
-      <c r="F3" s="47">
+      <c r="F3" s="43">
         <f>(D3*A3)+E3</f>
         <v>12.03</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="45">
+      <c r="H3" s="58" t="s">
+        <v>109</v>
+      </c>
+      <c r="I3" s="43">
+        <f>5*26</f>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A4" s="41">
         <v>3</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="47">
+      <c r="D4" s="43">
         <f>10.40833/A4</f>
         <v>3.469443333333333</v>
       </c>
-      <c r="E4" s="47">
+      <c r="E4" s="43">
         <f>3.25+2.73</f>
         <v>5.98</v>
       </c>
-      <c r="F4" s="47">
-        <f t="shared" ref="F4:F5" si="0">(D4*A4)+E4</f>
+      <c r="F4" s="43">
+        <f t="shared" ref="F4" si="0">(D4*A4)+E4</f>
         <v>16.38833</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A5" s="41">
         <v>3</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="47">
+      <c r="D5" s="43">
         <f>7.49/A5</f>
         <v>2.4966666666666666</v>
       </c>
-      <c r="E5" s="47">
+      <c r="E5" s="43">
         <f>3.15+2.15</f>
         <v>5.3</v>
       </c>
-      <c r="F5" s="47">
+      <c r="F5" s="43">
         <f>(D5*A5)+E5</f>
         <v>12.79</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="49">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A6" s="45">
         <v>1</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="50" t="s">
+      <c r="C6" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="D6" s="51">
+      <c r="D6" s="47">
         <v>16.13</v>
       </c>
-      <c r="E6" s="51">
+      <c r="E6" s="47">
         <f>F6-D6</f>
         <v>3.990000000000002</v>
       </c>
-      <c r="F6" s="51">
+      <c r="F6" s="47">
         <v>20.12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="54"/>
-      <c r="B7" s="54"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C8" s="52"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-    </row>
-    <row r="9" spans="1:6" s="41" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="57" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A7" s="48"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+    </row>
+    <row r="9" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="51" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="51" t="s">
         <v>105</v>
       </c>
-      <c r="D9" s="57" t="s">
+      <c r="F9" s="51" t="s">
         <v>106</v>
       </c>
-      <c r="F9" s="57" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B10" s="48">
+      <c r="H9" s="51" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B10" s="44">
         <f>SUM(F3:F6)</f>
         <v>61.328329999999994</v>
       </c>
-      <c r="C10" s="52"/>
-      <c r="D10" s="47">
+      <c r="D10" s="43">
         <f>B10/3</f>
         <v>20.442776666666663</v>
       </c>
-      <c r="E10" s="53"/>
-      <c r="F10" s="47">
+      <c r="F10" s="43">
         <f>SUM(F3:F5)/3</f>
         <v>13.736109999999998</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C11" s="52"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C12" s="52"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="57" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F13" s="47">
+      <c r="H10" s="43">
+        <f>F13+SUM(I2:I3)</f>
+        <v>186.20832999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="H11" s="59" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="F12" s="51" t="s">
+        <v>107</v>
+      </c>
+      <c r="H12" s="43">
+        <f>H10/3</f>
+        <v>62.069443333333332</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="F13" s="43">
         <f>SUM(F3:F5)</f>
         <v>41.208329999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="H14" s="59" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="H15" s="43">
+        <f>B10+SUM(I2:I3)</f>
+        <v>206.32832999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="H16" s="59" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.4">
+      <c r="H17" s="43">
+        <f>H15/3</f>
+        <v>68.776110000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added PDFs, Images and first few Theory parts #74
</commit_message>
<xml_diff>
--- a/Diplomarbeit/doc/Kampl/Hardware.xlsx
+++ b/Diplomarbeit/doc/Kampl/Hardware.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\Contrude\Diplomarbeit\doc\Kampl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maximilian\Desktop\Contrude\Diplomarbeit\doc\Kampl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92FAE9EE-698C-42CB-98AF-9DC302855487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46735563-C3D7-4218-874E-A997B6971DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="5" xr2:uid="{F8F58720-A04D-47BF-B44C-22AB8B67CE72}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="16200" activeTab="5" xr2:uid="{F8F58720-A04D-47BF-B44C-22AB8B67CE72}"/>
   </bookViews>
   <sheets>
     <sheet name="Anforderungen" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="114">
   <si>
     <t>Auflagen</t>
   </si>
@@ -262,9 +262,6 @@
     <t>Sehr Gut</t>
   </si>
   <si>
-    <t>3 Achsen Beschleunigungssensor</t>
-  </si>
-  <si>
     <t>Stromverbrauch</t>
   </si>
   <si>
@@ -383,6 +380,9 @@
   </si>
   <si>
     <t>Preis ins.</t>
+  </si>
+  <si>
+    <t>Lochrasterplatinen</t>
   </si>
 </sst>
 </file>
@@ -390,8 +390,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -673,7 +673,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="60">
@@ -682,23 +682,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -716,22 +716,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -741,13 +743,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Link" xfId="2" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Währung" xfId="1" builtinId="4"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -765,7 +765,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1719,7 +1719,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2039,39 +2039,39 @@
   <dimension ref="B2:K20"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="95" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" customWidth="1"/>
-    <col min="2" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.88671875" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="31.8" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B2" s="55" t="s">
+    <row r="2" spans="2:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="57"/>
-    </row>
-    <row r="3" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="59"/>
+    </row>
+    <row r="3" spans="2:11" ht="24" x14ac:dyDescent="0.4">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
@@ -2168,7 +2168,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
@@ -2296,14 +2296,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G10" s="7"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D12" s="11"/>
     </row>
-    <row r="13" spans="2:11" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="13" spans="2:11" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
@@ -2315,11 +2315,8 @@
       <c r="J13" s="18"/>
       <c r="K13" s="18"/>
     </row>
-    <row r="14" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:11" ht="24" x14ac:dyDescent="0.4">
       <c r="B14" s="12"/>
-      <c r="C14" t="s">
-        <v>73</v>
-      </c>
       <c r="D14" s="13"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
@@ -2329,21 +2326,21 @@
       <c r="J14" s="14"/>
       <c r="K14" s="12"/>
     </row>
-    <row r="15" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B15" s="15"/>
       <c r="C15" s="16"/>
       <c r="D15" s="17"/>
       <c r="F15" s="16"/>
       <c r="I15" s="16"/>
     </row>
-    <row r="16" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B16" s="15"/>
       <c r="C16" s="16"/>
       <c r="D16" s="17"/>
       <c r="F16" s="16"/>
       <c r="I16" s="16"/>
     </row>
-    <row r="17" spans="2:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B17" s="15"/>
       <c r="C17" s="16"/>
       <c r="D17" s="17"/>
@@ -2351,7 +2348,7 @@
       <c r="I17" s="16"/>
       <c r="J17" s="17"/>
     </row>
-    <row r="18" spans="2:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B18" s="15"/>
       <c r="C18" s="16"/>
       <c r="D18" s="17"/>
@@ -2359,7 +2356,7 @@
       <c r="I18" s="16"/>
       <c r="J18" s="17"/>
     </row>
-    <row r="19" spans="2:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B19" s="15"/>
       <c r="C19" s="16"/>
       <c r="D19" s="17"/>
@@ -2367,7 +2364,7 @@
       <c r="I19" s="16"/>
       <c r="J19" s="17"/>
     </row>
-    <row r="20" spans="2:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B20" s="15"/>
       <c r="C20" s="16"/>
       <c r="D20" s="17"/>
@@ -2409,33 +2406,33 @@
   <dimension ref="B1:XFD43"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="157" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F3" sqref="F3:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.44140625" style="22" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" style="22" customWidth="1"/>
     <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6 16384:16384" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:5 16384:16384" x14ac:dyDescent="0.25">
       <c r="B1" s="24" t="s">
         <v>43</v>
       </c>
@@ -2447,7 +2444,7 @@
       </c>
       <c r="E1" s="19"/>
     </row>
-    <row r="2" spans="2:6 16384:16384" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5 16384:16384" x14ac:dyDescent="0.25">
       <c r="B2" s="1">
         <v>1</v>
       </c>
@@ -2461,7 +2458,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5 16384:16384" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D3" s="23" t="s">
         <v>13</v>
       </c>
@@ -2469,60 +2466,48 @@
         <f xml:space="preserve"> 9.9+3.99</f>
         <v>13.89</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
       <c r="XFD3" s="10">
         <f t="shared" ref="XFD3:XFD8" si="0">SUM(E3:XFC3)</f>
-        <v>14.89</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>13.89</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5 16384:16384" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D4" s="23" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="8">
         <v>1.1100000000000001</v>
       </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
       <c r="XFD4" s="10">
         <f t="shared" si="0"/>
-        <v>4.1100000000000003</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5 16384:16384" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D5" s="23" t="s">
         <v>31</v>
       </c>
       <c r="E5" s="8">
         <v>2.72</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
       <c r="XFD5" s="10">
         <f t="shared" si="0"/>
-        <v>3.72</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.3">
+        <v>2.72</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5 16384:16384" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D6" s="23" t="s">
         <v>22</v>
       </c>
       <c r="E6" s="6">
         <v>5.9</v>
       </c>
-      <c r="F6">
-        <v>3</v>
-      </c>
       <c r="XFD6" s="10">
         <f t="shared" si="0"/>
-        <v>8.9</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6 16384:16384" x14ac:dyDescent="0.3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5 16384:16384" x14ac:dyDescent="0.25">
       <c r="D7" s="22" t="s">
         <v>41</v>
       </c>
@@ -2535,7 +2520,7 @@
         <v>23.619999999999997</v>
       </c>
     </row>
-    <row r="8" spans="2:6 16384:16384" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5 16384:16384" x14ac:dyDescent="0.25">
       <c r="D8" s="22" t="s">
         <v>40</v>
       </c>
@@ -2548,7 +2533,7 @@
         <v>70.859999999999985</v>
       </c>
     </row>
-    <row r="9" spans="2:6 16384:16384" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5 16384:16384" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>2</v>
       </c>
@@ -2562,7 +2547,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5 16384:16384" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C10" s="21"/>
       <c r="D10" s="23" t="s">
         <v>13</v>
@@ -2572,7 +2557,7 @@
         <v>13.89</v>
       </c>
     </row>
-    <row r="11" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5 16384:16384" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D11" s="4" t="s">
         <v>51</v>
       </c>
@@ -2580,7 +2565,7 @@
         <v>9.06</v>
       </c>
     </row>
-    <row r="12" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5 16384:16384" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D12" s="23" t="s">
         <v>31</v>
       </c>
@@ -2588,7 +2573,7 @@
         <v>2.72</v>
       </c>
     </row>
-    <row r="13" spans="2:6 16384:16384" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5 16384:16384" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D13" s="23" t="s">
         <v>22</v>
       </c>
@@ -2596,7 +2581,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="14" spans="2:6 16384:16384" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5 16384:16384" x14ac:dyDescent="0.25">
       <c r="D14" s="22" t="s">
         <v>41</v>
       </c>
@@ -2605,7 +2590,7 @@
         <v>31.57</v>
       </c>
     </row>
-    <row r="15" spans="2:6 16384:16384" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5 16384:16384" x14ac:dyDescent="0.25">
       <c r="D15" s="22" t="s">
         <v>40</v>
       </c>
@@ -2614,7 +2599,7 @@
         <v>94.710000000000008</v>
       </c>
     </row>
-    <row r="16" spans="2:6 16384:16384" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5 16384:16384" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>3</v>
       </c>
@@ -2628,7 +2613,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D17" s="4" t="s">
         <v>18</v>
       </c>
@@ -2636,7 +2621,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="18" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D18" s="23" t="s">
         <v>16</v>
       </c>
@@ -2644,7 +2629,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="19" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D19" s="23" t="s">
         <v>31</v>
       </c>
@@ -2652,7 +2637,7 @@
         <v>2.72</v>
       </c>
     </row>
-    <row r="20" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D20" s="23" t="s">
         <v>22</v>
       </c>
@@ -2660,7 +2645,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D21" s="22" t="s">
         <v>41</v>
       </c>
@@ -2669,7 +2654,7 @@
         <v>26.229999999999997</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D22" s="22" t="s">
         <v>40</v>
       </c>
@@ -2678,7 +2663,7 @@
         <v>78.69</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>4</v>
       </c>
@@ -2692,7 +2677,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D24" s="4" t="s">
         <v>18</v>
       </c>
@@ -2700,7 +2685,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="25" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D25" s="4" t="s">
         <v>51</v>
       </c>
@@ -2708,7 +2693,7 @@
         <v>9.06</v>
       </c>
     </row>
-    <row r="26" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D26" s="23" t="s">
         <v>31</v>
       </c>
@@ -2716,7 +2701,7 @@
         <v>2.72</v>
       </c>
     </row>
-    <row r="27" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D27" s="23" t="s">
         <v>22</v>
       </c>
@@ -2724,7 +2709,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D28" s="22" t="s">
         <v>41</v>
       </c>
@@ -2733,7 +2718,7 @@
         <v>34.18</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D29" s="22" t="s">
         <v>40</v>
       </c>
@@ -2742,7 +2727,7 @@
         <v>102.53999999999999</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>5</v>
       </c>
@@ -2756,7 +2741,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D31" s="4" t="s">
         <v>36</v>
       </c>
@@ -2764,7 +2749,7 @@
         <v>29.75</v>
       </c>
     </row>
-    <row r="32" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D32" s="4" t="s">
         <v>16</v>
       </c>
@@ -2772,7 +2757,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="33" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D33" s="23" t="s">
         <v>31</v>
       </c>
@@ -2780,7 +2765,7 @@
         <v>2.72</v>
       </c>
     </row>
-    <row r="34" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D34" s="23" t="s">
         <v>22</v>
       </c>
@@ -2788,7 +2773,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D35" s="22" t="s">
         <v>41</v>
       </c>
@@ -2797,7 +2782,7 @@
         <v>39.479999999999997</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D36" s="22" t="s">
         <v>40</v>
       </c>
@@ -2806,7 +2791,7 @@
         <v>118.44</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="1">
         <v>6</v>
       </c>
@@ -2820,7 +2805,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D38" s="4" t="s">
         <v>36</v>
       </c>
@@ -2828,7 +2813,7 @@
         <v>29.75</v>
       </c>
     </row>
-    <row r="39" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D39" s="4" t="s">
         <v>51</v>
       </c>
@@ -2836,7 +2821,7 @@
         <v>9.06</v>
       </c>
     </row>
-    <row r="40" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D40" s="23" t="s">
         <v>31</v>
       </c>
@@ -2844,7 +2829,7 @@
         <v>2.72</v>
       </c>
     </row>
-    <row r="41" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D41" s="23" t="s">
         <v>22</v>
       </c>
@@ -2852,7 +2837,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D42" s="22" t="s">
         <v>41</v>
       </c>
@@ -2861,7 +2846,7 @@
         <v>47.43</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D43" s="22" t="s">
         <v>40</v>
       </c>
@@ -2906,47 +2891,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56374579-2866-471D-B3A1-5191C1903E48}">
   <dimension ref="A2:J18"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="183" zoomScaleNormal="177" workbookViewId="0">
+    <sheetView zoomScale="183" zoomScaleNormal="177" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="19.44140625" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>13</v>
@@ -2962,7 +2947,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
@@ -2982,10 +2967,10 @@
       <c r="I5"/>
       <c r="J5" s="36"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C6" s="1">
         <v>5</v>
@@ -2998,10 +2983,10 @@
         <v>2.5999999999999998E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C7">
         <v>3.46</v>
@@ -3014,89 +2999,89 @@
         <v>1.384E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E8">
         <f>SUM(E4:E7)</f>
         <v>0.9991000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E9">
         <v>0.2</v>
       </c>
       <c r="F9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B11">
         <f>(E8)/1000</f>
         <v>9.9910000000000016E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B12">
         <f>(E8*24)/1000</f>
         <v>2.39784E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B13">
         <f>(E8*24*7)/1000</f>
         <v>0.16784880000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B14">
         <f>(E8*24*30)/1000</f>
         <v>0.71935199999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B16">
         <v>170</v>
       </c>
       <c r="C16" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B17">
         <f>B16/E9</f>
         <v>850</v>
       </c>
       <c r="C17" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18">
         <f>B17/24</f>
         <v>35.416666666666664</v>
       </c>
       <c r="C18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -3112,13 +3097,13 @@
       <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="30" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
         <v>53</v>
       </c>
@@ -3132,7 +3117,7 @@
       <c r="E1" s="32"/>
       <c r="F1" s="32"/>
     </row>
-    <row r="2" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>52</v>
       </c>
@@ -3152,7 +3137,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>54</v>
       </c>
@@ -3164,7 +3149,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>56</v>
       </c>
@@ -3176,7 +3161,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>57</v>
       </c>
@@ -3188,7 +3173,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>58</v>
       </c>
@@ -3200,7 +3185,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>61</v>
       </c>
@@ -3212,13 +3197,13 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
         <v>62</v>
       </c>
       <c r="B9" s="34"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -3226,7 +3211,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -3234,7 +3219,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>3</v>
       </c>
@@ -3242,7 +3227,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>4</v>
       </c>
@@ -3250,7 +3235,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>5</v>
       </c>
@@ -3258,7 +3243,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>6</v>
       </c>
@@ -3266,7 +3251,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>7</v>
       </c>
@@ -3274,7 +3259,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>8</v>
       </c>
@@ -3282,7 +3267,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>9</v>
       </c>
@@ -3290,7 +3275,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>10</v>
       </c>
@@ -3309,24 +3294,24 @@
   <dimension ref="A5:A7"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -3340,61 +3325,62 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493E053C-96E9-4B54-B663-4984A59DE940}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.5546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" style="37" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" style="40" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" style="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35" style="40" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" style="37"/>
-    <col min="8" max="8" width="22.5546875" style="37" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.44140625" style="37"/>
+    <col min="1" max="1" width="9.5703125" style="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" style="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" style="37" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" style="40" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.28515625" style="40" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="37"/>
+    <col min="8" max="8" width="27.28515625" style="37" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" style="37" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" style="37" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F1" s="39"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="53" t="s">
         <v>97</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="C2" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="53" t="s">
-        <v>99</v>
-      </c>
       <c r="D2" s="54" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="54" t="s">
         <v>101</v>
       </c>
-      <c r="E2" s="54" t="s">
+      <c r="F2" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="F2" s="54" t="s">
-        <v>103</v>
-      </c>
-      <c r="H2" s="58" t="s">
-        <v>108</v>
+      <c r="H2" s="55" t="s">
+        <v>107</v>
       </c>
       <c r="I2" s="43">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="41">
         <v>3</v>
       </c>
       <c r="B3" s="42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C3" s="42" t="s">
         <v>16</v>
@@ -3410,23 +3396,23 @@
         <f>(D3*A3)+E3</f>
         <v>12.03</v>
       </c>
-      <c r="H3" s="58" t="s">
-        <v>109</v>
+      <c r="H3" s="55" t="s">
+        <v>108</v>
       </c>
       <c r="I3" s="43">
         <f>5*26</f>
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="41">
         <v>3</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D4" s="43">
         <f>10.40833/A4</f>
@@ -3437,137 +3423,164 @@
         <v>5.98</v>
       </c>
       <c r="F4" s="43">
-        <f t="shared" ref="F4" si="0">(D4*A4)+E4</f>
+        <f>(D4*A4)+E4</f>
         <v>16.38833</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="41">
+        <v>32</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="43">
+        <v>13.21</v>
+      </c>
+      <c r="E5" s="43">
+        <v>6.65</v>
+      </c>
+      <c r="F5" s="43">
+        <f>D5+E5</f>
+        <v>19.86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="41">
         <v>3</v>
       </c>
-      <c r="B5" s="41" t="s">
-        <v>96</v>
-      </c>
-      <c r="C5" s="42" t="s">
+      <c r="B6" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="43">
-        <f>7.49/A5</f>
+      <c r="C6" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="43">
+        <f>7.49/A6</f>
         <v>2.4966666666666666</v>
       </c>
-      <c r="E5" s="43">
+      <c r="E6" s="43">
         <f>3.15+2.15</f>
         <v>5.3</v>
       </c>
-      <c r="F5" s="43">
-        <f>(D5*A5)+E5</f>
+      <c r="F6" s="43">
+        <f>(D6*A6)+E6</f>
         <v>12.79</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A6" s="45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="45">
         <v>1</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B7" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C7" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="47">
+        <v>16.13</v>
+      </c>
+      <c r="E7" s="47">
+        <f>F7-D7</f>
+        <v>3.990000000000002</v>
+      </c>
+      <c r="F7" s="47">
+        <v>20.12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="48"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+    </row>
+    <row r="10" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="51" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="51" t="s">
         <v>104</v>
       </c>
-      <c r="D6" s="47">
-        <v>16.13</v>
-      </c>
-      <c r="E6" s="47">
-        <f>F6-D6</f>
-        <v>3.990000000000002</v>
-      </c>
-      <c r="F6" s="47">
-        <v>20.12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A7" s="48"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-    </row>
-    <row r="9" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="51" t="s">
+      <c r="F10" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="H10" s="51" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B11" s="44">
+        <f>SUM(F3:F7)</f>
+        <v>81.188329999999993</v>
+      </c>
+      <c r="D11" s="43">
+        <f>B11/3</f>
+        <v>27.062776666666664</v>
+      </c>
+      <c r="F11" s="43">
+        <f>SUM(F3:F6)/3</f>
+        <v>20.356109999999997</v>
+      </c>
+      <c r="H11" s="43">
+        <f>SUM(F3:F6)</f>
+        <v>61.068329999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B16" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="D9" s="51" t="s">
-        <v>105</v>
-      </c>
-      <c r="F9" s="51" t="s">
-        <v>106</v>
-      </c>
-      <c r="H9" s="51" t="s">
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B17" s="43">
+        <f>H11+SUM(I2:I3)</f>
+        <v>206.06833</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B18" s="56" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B10" s="44">
-        <f>SUM(F3:F6)</f>
-        <v>61.328329999999994</v>
-      </c>
-      <c r="D10" s="43">
-        <f>B10/3</f>
-        <v>20.442776666666663</v>
-      </c>
-      <c r="F10" s="43">
-        <f>SUM(F3:F5)/3</f>
-        <v>13.736109999999998</v>
-      </c>
-      <c r="H10" s="43">
-        <f>F13+SUM(I2:I3)</f>
-        <v>186.20832999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="H11" s="59" t="s">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B19" s="43">
+        <f>B17/3</f>
+        <v>68.68944333333333</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B20" s="37"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B21" s="56" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="F12" s="51" t="s">
-        <v>107</v>
-      </c>
-      <c r="H12" s="43">
-        <f>H10/3</f>
-        <v>62.069443333333332</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="F13" s="43">
-        <f>SUM(F3:F5)</f>
-        <v>41.208329999999997</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="H14" s="59" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="H15" s="43">
-        <f>B10+SUM(I2:I3)</f>
-        <v>206.32832999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="H16" s="59" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.4">
-      <c r="H17" s="43">
-        <f>H15/3</f>
-        <v>68.776110000000003</v>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B22" s="43">
+        <f>B11+SUM(I2:I3)</f>
+        <v>226.18833000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B23" s="56" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B24" s="43">
+        <f>B22/3</f>
+        <v>75.396110000000007</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>